<commit_message>
updated VGGT16.1d South Africa and VGGT16.1e Rwanda values
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/NKT-VGGT16/NKT-VGGT16.xlsx
+++ b/Simple_XLS_Importer/data/NKT-VGGT16/NKT-VGGT16.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\vm\debian8.2-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\landbook-importers\Simple_XLS_Importer\data\NKT-VGGT16\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1114,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B145" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3137,8 +3137,8 @@
       <c r="C112" s="4">
         <v>2016</v>
       </c>
-      <c r="D112" s="8" t="s">
-        <v>52</v>
+      <c r="D112" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="E112" s="20" t="s">
         <v>189</v>
@@ -3662,8 +3662,8 @@
       <c r="C141" s="4">
         <v>2016</v>
       </c>
-      <c r="D141" s="7" t="s">
-        <v>54</v>
+      <c r="D141" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="E141" s="20" t="s">
         <v>122</v>

</xml_diff>